<commit_message>
Add eq to measurements
</commit_message>
<xml_diff>
--- a/source/sensor/measurements/measurements_ir.xlsx
+++ b/source/sensor/measurements/measurements_ir.xlsx
@@ -1,16 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\LiTHe-Hex\source\sensor\measurements\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="996" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="996"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -22,45 +26,27 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t xml:space="preserve">Längd (cm)</t>
+    <t>Längd (cm)</t>
   </si>
   <si>
-    <t xml:space="preserve">Värde</t>
+    <t>Värde</t>
   </si>
   <si>
-    <t xml:space="preserve">Medel</t>
+    <t>Medel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -75,7 +61,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -83,53 +69,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -188,17 +140,37 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
+  <c:style val="2"/>
   <c:chart>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
+      <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -217,9 +189,6 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
             <a:ln w="28800">
               <a:noFill/>
             </a:ln>
@@ -234,13 +203,41 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
+          <c:trendline>
+            <c:trendlineType val="poly"/>
+            <c:order val="4"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="3.8069230241963126E-2"/>
+                  <c:y val="8.4584225055054127E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$A$2:$A$15</c:f>
@@ -320,7 +317,7 @@
                   <c:v>153.4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>137.2</c:v>
+                  <c:v>137.19999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>124.4</c:v>
@@ -345,11 +342,19 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="61916734"/>
-        <c:axId val="827089"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="234319112"/>
+        <c:axId val="234316368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="61916734"/>
+        <c:axId val="234319112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -362,34 +367,36 @@
         <c:spPr>
           <a:ln>
             <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
+              <a:srgbClr val="B3B3B3"/>
             </a:solidFill>
           </a:ln>
         </c:spPr>
         <c:txPr>
           <a:bodyPr/>
+          <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
                 <a:uFill>
                   <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a:uFill>
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="827089"/>
+        <c:crossAx val="234316368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="827089"/>
+        <c:axId val="234316368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -399,7 +406,7 @@
           <c:spPr>
             <a:ln>
               <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
+                <a:srgbClr val="B3B3B3"/>
               </a:solidFill>
             </a:ln>
           </c:spPr>
@@ -411,29 +418,31 @@
         <c:spPr>
           <a:ln>
             <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
+              <a:srgbClr val="B3B3B3"/>
             </a:solidFill>
           </a:ln>
         </c:spPr>
         <c:txPr>
           <a:bodyPr/>
+          <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
                 <a:uFill>
                   <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a:uFill>
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61916734"/>
+        <c:crossAx val="234319112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -441,13 +450,14 @@
         <a:noFill/>
         <a:ln>
           <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
+            <a:srgbClr val="B3B3B3"/>
           </a:solidFill>
         </a:ln>
       </c:spPr>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -458,20 +468,26 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="span"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:srgbClr val="ffffff"/>
+      <a:srgbClr val="FFFFFF"/>
     </a:solidFill>
     <a:ln>
       <a:noFill/>
     </a:ln>
   </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
@@ -485,14 +501,14 @@
       <xdr:row>21</xdr:row>
       <xdr:rowOff>81360</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="0" name=""/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7315200" y="258120"/>
-        <a:ext cx="5759640" cy="3236760"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -505,370 +521,628 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I29" activeCellId="0" sqref="I29"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col min="1" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="1" t="s">
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
         <v>20</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2">
         <v>505</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2">
         <v>510</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2">
         <v>505</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2">
         <v>510</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2">
         <v>504</v>
       </c>
-      <c r="G2" s="1" t="n">
-        <f aca="false">AVERAGE(B2:F2)</f>
+      <c r="G2" s="2">
+        <f t="shared" ref="G2:G15" si="0">AVERAGE(B2:F2)</f>
         <v>506.8</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
         <v>30</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3">
         <v>390</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3">
         <v>395</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3">
         <v>394</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3">
         <v>391</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3">
         <v>391</v>
       </c>
-      <c r="G3" s="1" t="n">
-        <f aca="false">AVERAGE(B3:F3)</f>
+      <c r="G3" s="2">
+        <f t="shared" si="0"/>
         <v>392.2</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
         <v>40</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4">
         <v>300</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4">
         <v>301</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4">
         <v>300</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4">
         <v>303</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4">
         <v>300</v>
       </c>
-      <c r="G4" s="1" t="n">
-        <f aca="false">AVERAGE(B4:F4)</f>
+      <c r="G4" s="2">
+        <f t="shared" si="0"/>
         <v>300.8</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
         <v>50</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5">
         <v>239</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5">
         <v>243</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5">
         <v>246</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5">
         <v>246</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5">
         <v>243</v>
       </c>
-      <c r="G5" s="1" t="n">
-        <f aca="false">AVERAGE(B5:F5)</f>
+      <c r="G5" s="2">
+        <f t="shared" si="0"/>
         <v>243.4</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
         <v>60</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6">
         <v>207</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6">
         <v>207</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6">
         <v>209</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6">
         <v>204</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6">
         <v>200</v>
       </c>
-      <c r="G6" s="1" t="n">
-        <f aca="false">AVERAGE(B6:F6)</f>
+      <c r="G6" s="2">
+        <f t="shared" si="0"/>
         <v>205.4</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
         <v>70</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7">
         <v>173</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7">
         <v>174</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7">
         <v>176</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7">
         <v>173</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F7">
         <v>174</v>
       </c>
-      <c r="G7" s="1" t="n">
-        <f aca="false">AVERAGE(B7:F7)</f>
+      <c r="G7" s="2">
+        <f t="shared" si="0"/>
         <v>174</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
         <v>80</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8">
         <v>152</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8">
         <v>156</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8">
         <v>155</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8">
         <v>152</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="F8">
         <v>152</v>
       </c>
-      <c r="G8" s="1" t="n">
-        <f aca="false">AVERAGE(B8:F8)</f>
+      <c r="G8" s="2">
+        <f t="shared" si="0"/>
         <v>153.4</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
         <v>90</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9">
         <v>136</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9">
         <v>140</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9">
         <v>135</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9">
         <v>135</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="F9">
         <v>140</v>
       </c>
-      <c r="G9" s="1" t="n">
-        <f aca="false">AVERAGE(B9:F9)</f>
-        <v>137.2</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="n">
+      <c r="G9" s="2">
+        <f t="shared" si="0"/>
+        <v>137.19999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
         <v>100</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10">
         <v>126</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10">
         <v>122</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10">
         <v>126</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10">
         <v>121</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="F10">
         <v>127</v>
       </c>
-      <c r="G10" s="1" t="n">
-        <f aca="false">AVERAGE(B10:F10)</f>
+      <c r="G10" s="2">
+        <f t="shared" si="0"/>
         <v>124.4</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="n">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
         <v>110</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11">
         <v>113</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11">
         <v>112</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11">
         <v>113</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11">
         <v>112</v>
       </c>
-      <c r="F11" s="0" t="n">
+      <c r="F11">
         <v>112</v>
       </c>
-      <c r="G11" s="1" t="n">
-        <f aca="false">AVERAGE(B11:F11)</f>
+      <c r="G11" s="2">
+        <f t="shared" si="0"/>
         <v>112.4</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="n">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
         <v>120</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12">
         <v>105</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12">
         <v>104</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="D12">
         <v>103</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E12">
         <v>104</v>
       </c>
-      <c r="F12" s="0" t="n">
+      <c r="F12">
         <v>104</v>
       </c>
-      <c r="G12" s="1" t="n">
-        <f aca="false">AVERAGE(B12:F12)</f>
+      <c r="G12" s="2">
+        <f t="shared" si="0"/>
         <v>104</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="n">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
         <v>130</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B13">
         <v>97</v>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="C13">
         <v>96</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="D13">
         <v>95</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="E13">
         <v>95</v>
       </c>
-      <c r="F13" s="0" t="n">
+      <c r="F13">
         <v>95</v>
       </c>
-      <c r="G13" s="1" t="n">
-        <f aca="false">AVERAGE(B13:F13)</f>
+      <c r="G13" s="2">
+        <f t="shared" si="0"/>
         <v>95.6</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="n">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
         <v>140</v>
       </c>
-      <c r="B14" s="0" t="n">
+      <c r="B14">
         <v>89</v>
       </c>
-      <c r="C14" s="0" t="n">
+      <c r="C14">
         <v>87</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="D14">
         <v>87</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="E14">
         <v>86</v>
       </c>
-      <c r="F14" s="0" t="n">
+      <c r="F14">
         <v>88</v>
       </c>
-      <c r="G14" s="1" t="n">
-        <f aca="false">AVERAGE(B14:F14)</f>
+      <c r="G14" s="2">
+        <f t="shared" si="0"/>
         <v>87.4</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="n">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
         <v>150</v>
       </c>
-      <c r="B15" s="0" t="n">
+      <c r="B15">
         <v>83</v>
       </c>
-      <c r="C15" s="0" t="n">
+      <c r="C15">
         <v>83</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="D15">
         <v>83</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="E15">
         <v>85</v>
       </c>
-      <c r="F15" s="0" t="n">
+      <c r="F15">
         <v>83</v>
       </c>
-      <c r="G15" s="1" t="n">
-        <f aca="false">AVERAGE(B15:F15)</f>
+      <c r="G15" s="2">
+        <f t="shared" si="0"/>
         <v>83.4</v>
       </c>
     </row>
@@ -876,10 +1150,9 @@
   <mergeCells count="1">
     <mergeCell ref="B1:F1"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Get sensor data in meter
</commit_message>
<xml_diff>
--- a/source/sensor/measurements/measurements_ir.xlsx
+++ b/source/sensor/measurements/measurements_ir.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
   <si>
     <t>Längd (cm)</t>
   </si>
@@ -39,7 +39,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -48,6 +48,12 @@
     <font>
       <b/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF595959"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -72,10 +78,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -166,9 +175,47 @@
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
-  <c:style val="2"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -189,56 +236,129 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28800">
+            <a:ln w="19050" cap="rnd">
               <a:noFill/>
+              <a:round/>
             </a:ln>
+            <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="8"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="004586"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="1"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="0"/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
+          </c:marker>
           <c:trendline>
-            <c:trendlineType val="poly"/>
-            <c:order val="4"/>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="3.8069230241963126E-2"/>
-                  <c:y val="8.4584225055054127E-2"/>
+                  <c:x val="-0.26002143482064743"/>
+                  <c:y val="3.0395158938465176E-3"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$2:$G$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>506.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>392.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>243.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>205.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>174</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>153.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>137.19999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>124.4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>112.4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>95.6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>87.4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>83.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Sheet1!$A$2:$A$15</c:f>
               <c:numCache>
@@ -285,57 +405,6 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>150</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$G$2:$G$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>506.8</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>392.2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>300.8</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>243.4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>205.4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>174</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>153.4</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>137.19999999999999</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>124.4</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>112.4</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>104</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>95.6</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>87.4</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>83.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -350,53 +419,73 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="234319112"/>
-        <c:axId val="234316368"/>
+        <c:axId val="204285272"/>
+        <c:axId val="506824144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="234319112"/>
+        <c:axId val="204285272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:srgbClr val="B3B3B3"/>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
             </a:solidFill>
+            <a:round/>
           </a:ln>
+          <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:srgbClr val="000000"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
                 </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Arial"/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="234316368"/>
+        <c:crossAx val="506824144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="234316368"/>
+        <c:axId val="506824144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -404,80 +493,96 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:ln>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:srgbClr val="B3B3B3"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
               </a:solidFill>
+              <a:round/>
             </a:ln>
+            <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:srgbClr val="B3B3B3"/>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
             </a:solidFill>
+            <a:round/>
           </a:ln>
+          <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:srgbClr val="000000"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
                 </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Arial"/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="234319112"/>
+        <c:crossAx val="204285272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="B3B3B3"/>
-          </a:solidFill>
+          <a:noFill/>
         </a:ln>
+        <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="span"/>
-    <c:showDLblsOverMax val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:srgbClr val="FFFFFF"/>
+      <a:schemeClr val="bg1"/>
     </a:solidFill>
-    <a:ln>
-      <a:noFill/>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
     </a:ln>
+    <a:effectLst/>
   </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -486,24 +591,1589 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Medel</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.32359339457567804"/>
+                  <c:y val="-1.980169145523476E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$23:$G$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>551.79999999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>403</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>312.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>249.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>210.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>180.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>157.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>141.19999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>122.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>111.4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>103.4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>88.4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>78.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$23:$A$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="204284880"/>
+        <c:axId val="508052344"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="204284880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="508052344"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="508052344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="204284880"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>95760</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>70200</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="5" name="Chart 4"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -513,6 +2183,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>52387</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>766762</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -784,10 +2484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K35" sqref="K35"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -796,22 +2496,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="2" t="s">
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
+      <c r="A2" s="1">
         <v>20</v>
       </c>
       <c r="B2">
@@ -829,13 +2529,13 @@
       <c r="F2">
         <v>504</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="1">
         <f t="shared" ref="G2:G15" si="0">AVERAGE(B2:F2)</f>
         <v>506.8</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>30</v>
       </c>
       <c r="B3">
@@ -853,13 +2553,13 @@
       <c r="F3">
         <v>391</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="1">
         <f t="shared" si="0"/>
         <v>392.2</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>40</v>
       </c>
       <c r="B4">
@@ -877,13 +2577,13 @@
       <c r="F4">
         <v>300</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="1">
         <f t="shared" si="0"/>
         <v>300.8</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>50</v>
       </c>
       <c r="B5">
@@ -901,13 +2601,13 @@
       <c r="F5">
         <v>243</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="1">
         <f t="shared" si="0"/>
         <v>243.4</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>60</v>
       </c>
       <c r="B6">
@@ -925,13 +2625,13 @@
       <c r="F6">
         <v>200</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="1">
         <f t="shared" si="0"/>
         <v>205.4</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
+      <c r="A7" s="1">
         <v>70</v>
       </c>
       <c r="B7">
@@ -949,13 +2649,13 @@
       <c r="F7">
         <v>174</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="1">
         <f t="shared" si="0"/>
         <v>174</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
+      <c r="A8" s="1">
         <v>80</v>
       </c>
       <c r="B8">
@@ -973,13 +2673,13 @@
       <c r="F8">
         <v>152</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="1">
         <f t="shared" si="0"/>
         <v>153.4</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
+      <c r="A9" s="1">
         <v>90</v>
       </c>
       <c r="B9">
@@ -997,13 +2697,13 @@
       <c r="F9">
         <v>140</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="1">
         <f t="shared" si="0"/>
         <v>137.19999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
+      <c r="A10" s="1">
         <v>100</v>
       </c>
       <c r="B10">
@@ -1021,13 +2721,13 @@
       <c r="F10">
         <v>127</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="1">
         <f t="shared" si="0"/>
         <v>124.4</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
+      <c r="A11" s="1">
         <v>110</v>
       </c>
       <c r="B11">
@@ -1045,13 +2745,13 @@
       <c r="F11">
         <v>112</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="1">
         <f t="shared" si="0"/>
         <v>112.4</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
+      <c r="A12" s="1">
         <v>120</v>
       </c>
       <c r="B12">
@@ -1069,13 +2769,13 @@
       <c r="F12">
         <v>104</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="1">
         <f t="shared" si="0"/>
         <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
+      <c r="A13" s="1">
         <v>130</v>
       </c>
       <c r="B13">
@@ -1093,13 +2793,13 @@
       <c r="F13">
         <v>95</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="1">
         <f t="shared" si="0"/>
         <v>95.6</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
+      <c r="A14" s="1">
         <v>140</v>
       </c>
       <c r="B14">
@@ -1117,13 +2817,13 @@
       <c r="F14">
         <v>88</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14" s="1">
         <f t="shared" si="0"/>
         <v>87.4</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
+      <c r="A15" s="1">
         <v>150</v>
       </c>
       <c r="B15">
@@ -1141,14 +2841,377 @@
       <c r="F15">
         <v>83</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="1">
         <f t="shared" si="0"/>
         <v>83.4</v>
       </c>
     </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>4</v>
+      </c>
+      <c r="B23">
+        <v>551</v>
+      </c>
+      <c r="C23">
+        <v>550</v>
+      </c>
+      <c r="D23">
+        <v>550</v>
+      </c>
+      <c r="E23">
+        <v>559</v>
+      </c>
+      <c r="F23">
+        <v>549</v>
+      </c>
+      <c r="G23">
+        <f>AVERAGE(B23:F23)</f>
+        <v>551.79999999999995</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>6</v>
+      </c>
+      <c r="B24">
+        <v>406</v>
+      </c>
+      <c r="C24">
+        <v>399</v>
+      </c>
+      <c r="D24">
+        <v>399</v>
+      </c>
+      <c r="E24">
+        <v>405</v>
+      </c>
+      <c r="F24">
+        <v>406</v>
+      </c>
+      <c r="G24">
+        <f t="shared" ref="G24:G36" si="1">AVERAGE(B24:F24)</f>
+        <v>403</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>8</v>
+      </c>
+      <c r="B25">
+        <v>315</v>
+      </c>
+      <c r="C25">
+        <v>310</v>
+      </c>
+      <c r="D25">
+        <v>310</v>
+      </c>
+      <c r="E25">
+        <v>315</v>
+      </c>
+      <c r="F25">
+        <v>311</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="1"/>
+        <v>312.2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>10</v>
+      </c>
+      <c r="B26">
+        <v>235</v>
+      </c>
+      <c r="C26">
+        <v>252</v>
+      </c>
+      <c r="D26">
+        <v>252</v>
+      </c>
+      <c r="E26">
+        <v>257</v>
+      </c>
+      <c r="F26">
+        <v>252</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="1"/>
+        <v>249.6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>12</v>
+      </c>
+      <c r="B27">
+        <v>210</v>
+      </c>
+      <c r="C27">
+        <v>210</v>
+      </c>
+      <c r="D27">
+        <v>209</v>
+      </c>
+      <c r="E27">
+        <v>210</v>
+      </c>
+      <c r="F27">
+        <v>212</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="1"/>
+        <v>210.2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>14</v>
+      </c>
+      <c r="B28">
+        <v>179</v>
+      </c>
+      <c r="C28">
+        <v>179</v>
+      </c>
+      <c r="D28">
+        <v>179</v>
+      </c>
+      <c r="E28">
+        <v>186</v>
+      </c>
+      <c r="F28">
+        <v>179</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="1"/>
+        <v>180.4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>16</v>
+      </c>
+      <c r="B29">
+        <v>155</v>
+      </c>
+      <c r="C29">
+        <v>159</v>
+      </c>
+      <c r="D29">
+        <v>156</v>
+      </c>
+      <c r="E29">
+        <v>159</v>
+      </c>
+      <c r="F29">
+        <v>159</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="1"/>
+        <v>157.6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>18</v>
+      </c>
+      <c r="B30">
+        <v>140</v>
+      </c>
+      <c r="C30">
+        <v>142</v>
+      </c>
+      <c r="D30">
+        <v>143</v>
+      </c>
+      <c r="E30">
+        <v>140</v>
+      </c>
+      <c r="F30">
+        <v>141</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="1"/>
+        <v>141.19999999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>20</v>
+      </c>
+      <c r="B31">
+        <v>122</v>
+      </c>
+      <c r="C31">
+        <v>123</v>
+      </c>
+      <c r="D31">
+        <v>123</v>
+      </c>
+      <c r="E31">
+        <v>123</v>
+      </c>
+      <c r="F31">
+        <v>123</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="1"/>
+        <v>122.8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>22</v>
+      </c>
+      <c r="B32">
+        <v>112</v>
+      </c>
+      <c r="C32">
+        <v>112</v>
+      </c>
+      <c r="D32">
+        <v>111</v>
+      </c>
+      <c r="E32">
+        <v>111</v>
+      </c>
+      <c r="F32">
+        <v>111</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="1"/>
+        <v>111.4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>24</v>
+      </c>
+      <c r="B33">
+        <v>103</v>
+      </c>
+      <c r="C33">
+        <v>105</v>
+      </c>
+      <c r="D33">
+        <v>103</v>
+      </c>
+      <c r="E33">
+        <v>103</v>
+      </c>
+      <c r="F33">
+        <v>103</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="1"/>
+        <v>103.4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>26</v>
+      </c>
+      <c r="B34">
+        <v>91</v>
+      </c>
+      <c r="C34">
+        <v>95</v>
+      </c>
+      <c r="D34">
+        <v>89</v>
+      </c>
+      <c r="E34">
+        <v>93</v>
+      </c>
+      <c r="F34">
+        <v>92</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="1"/>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>28</v>
+      </c>
+      <c r="B35">
+        <v>88</v>
+      </c>
+      <c r="C35">
+        <v>87</v>
+      </c>
+      <c r="D35">
+        <v>89</v>
+      </c>
+      <c r="E35">
+        <v>89</v>
+      </c>
+      <c r="F35">
+        <v>89</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="1"/>
+        <v>88.4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>30</v>
+      </c>
+      <c r="B36">
+        <v>79</v>
+      </c>
+      <c r="C36">
+        <v>76</v>
+      </c>
+      <c r="D36">
+        <v>81</v>
+      </c>
+      <c r="E36">
+        <v>79</v>
+      </c>
+      <c r="F36">
+        <v>76</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="1"/>
+        <v>78.2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C40">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="C42" s="3">
+        <f>0.0036 *C40^4 - 0.3094 *C40^3 + 9.8205 *C40^2 - 144.8*C40 + 987.88</f>
+        <v>7334113.8099999987</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B22:F22"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>